<commit_message>
Update 3th_Project_기능 정의서(수정) - 복사본.xlsx
</commit_message>
<xml_diff>
--- a/Text/01.기능정의서/3th_Project_기능 정의서(수정) - 복사본.xlsx
+++ b/Text/01.기능정의서/3th_Project_기능 정의서(수정) - 복사본.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="380" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="기능 정의서-1" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1532" uniqueCount="1532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="1534">
   <si>
     <t>번호</t>
   </si>
@@ -16058,6 +16058,26 @@
   </si>
   <si>
     <t>게시글답글</t>
+  </si>
+  <si>
+    <t>- 구매가 가능한 교재목록이 자동적으로 슬라이드
+- 마우스를 올릴 시 정지
+- 각 방향 쪽으로 이동시 그 방향으로 1장씩 슬라이드</t>
+  </si>
+  <si>
+    <r>
+      <t>- 구매</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>가 가능한 교재목록이 자동적으로 슬라이드
+- 마우스를 올릴 시 정지
+- 각 방향 쪽으로 이동시 그 방향으로 1장씩 슬라이드</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -17250,7 +17270,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="503">
+  <cellXfs count="504">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -18759,6 +18779,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="35" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -20514,8 +20537,8 @@
   <dimension ref="A1:R192"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.500000"/>
@@ -20617,8 +20640,8 @@
       </c>
       <c r="I3" s="311"/>
       <c r="J3" s="311"/>
-      <c r="K3" s="135" t="s">
-        <v>1206</v>
+      <c r="K3" s="503" t="s">
+        <v>1533</v>
       </c>
       <c r="L3" s="426"/>
       <c r="M3" s="426"/>

</xml_diff>